<commit_message>
ANOVA + posthoc analysis Updates to boxplot
</commit_message>
<xml_diff>
--- a/data/082023_Mapping.xlsx
+++ b/data/082023_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olegtutanov/Documents/Programming/Olink/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50CA1FCB-0621-8C42-B90E-D1C6843DC529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD0A70F-30F1-0942-8742-97A2FC2C0053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="-16020" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
+    <workbookView xWindow="5220" yWindow="-17440" windowWidth="25640" windowHeight="14440" xr2:uid="{2D7CE3BD-EF66-D84A-A92E-36ED3E223C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="94">
   <si>
     <t>SampleID</t>
   </si>
@@ -210,13 +210,121 @@
   </si>
   <si>
     <t>Experiment</t>
+  </si>
+  <si>
+    <t>Subset</t>
+  </si>
+  <si>
+    <t>Untreated</t>
+  </si>
+  <si>
+    <t>DiFi Supermere Day 0</t>
+  </si>
+  <si>
+    <t>DiFi Supermere Day 4</t>
+  </si>
+  <si>
+    <t>DiFi Supermere Day 2</t>
+  </si>
+  <si>
+    <t>CC-CR Supermere Day 0</t>
+  </si>
+  <si>
+    <t>CC-CR Supermere Day 2</t>
+  </si>
+  <si>
+    <t>CC-CR Supermere Day 4</t>
+  </si>
+  <si>
+    <t>DiFi Exomere Day 0</t>
+  </si>
+  <si>
+    <t>DiFi Exomere Day 2</t>
+  </si>
+  <si>
+    <t>DiFi Exomere Day 4</t>
+  </si>
+  <si>
+    <t>Supermere INPUT</t>
+  </si>
+  <si>
+    <t>Supermere MOCK</t>
+  </si>
+  <si>
+    <t>Supermere RNAse temp</t>
+  </si>
+  <si>
+    <t>RNAse temp</t>
+  </si>
+  <si>
+    <t>RNAse MOCK</t>
+  </si>
+  <si>
+    <t>DiFi Supermere</t>
+  </si>
+  <si>
+    <t>DiFi Supermere + TGFBI</t>
+  </si>
+  <si>
+    <t>DiFi Supermere TGFBI OE</t>
+  </si>
+  <si>
+    <t>TGFBI</t>
+  </si>
+  <si>
+    <t>DiFi FPLC Supermere</t>
+  </si>
+  <si>
+    <t>DiFi FPLC Exomere</t>
+  </si>
+  <si>
+    <t>DiFi UC Supermere</t>
+  </si>
+  <si>
+    <t>DiFi UC Exomere</t>
+  </si>
+  <si>
+    <t>DiFi UC sEV</t>
+  </si>
+  <si>
+    <t>CC-CR FPLC Supermere</t>
+  </si>
+  <si>
+    <t>CC-CR FPLC Exomere</t>
+  </si>
+  <si>
+    <t>CC-CR UC Supermere</t>
+  </si>
+  <si>
+    <t>CC-CR UC Exomere</t>
+  </si>
+  <si>
+    <t>CC-CR UC sEV</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>Healthy no cells</t>
+  </si>
+  <si>
+    <t>CRC no cells</t>
+  </si>
+  <si>
+    <t>Plasma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -228,6 +336,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -567,15 +681,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8942E758-F973-BE42-9C82-133C20AF9680}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,8 +699,11 @@
       <c r="C1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -596,8 +713,11 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -607,8 +727,11 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -618,8 +741,11 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -629,8 +755,11 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,8 +769,11 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -651,8 +783,11 @@
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -662,8 +797,11 @@
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,8 +811,11 @@
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -684,8 +825,11 @@
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -695,8 +839,11 @@
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,8 +853,11 @@
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -717,8 +867,11 @@
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -728,8 +881,11 @@
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -739,8 +895,11 @@
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -750,8 +909,11 @@
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -761,8 +923,11 @@
       <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -772,8 +937,11 @@
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -783,8 +951,11 @@
       <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -794,8 +965,11 @@
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -805,8 +979,11 @@
       <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -816,8 +993,11 @@
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -827,8 +1007,11 @@
       <c r="C23" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -838,8 +1021,11 @@
       <c r="C24" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -849,8 +1035,11 @@
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -860,8 +1049,11 @@
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -871,8 +1063,11 @@
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -882,8 +1077,11 @@
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -893,8 +1091,11 @@
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -904,8 +1105,11 @@
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -915,8 +1119,11 @@
       <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -926,8 +1133,11 @@
       <c r="C32" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -937,8 +1147,11 @@
       <c r="C33" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -948,8 +1161,11 @@
       <c r="C34" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -959,8 +1175,11 @@
       <c r="C35" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -970,8 +1189,11 @@
       <c r="C36" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -981,8 +1203,11 @@
       <c r="C37" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -992,8 +1217,11 @@
       <c r="C38" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1003,8 +1231,11 @@
       <c r="C39" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1014,8 +1245,11 @@
       <c r="C40" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -1025,8 +1259,11 @@
       <c r="C41" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -1036,8 +1273,11 @@
       <c r="C42" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1047,8 +1287,11 @@
       <c r="C43" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1056,10 +1299,13 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -1069,8 +1315,11 @@
       <c r="C45" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -1080,8 +1329,11 @@
       <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -1091,8 +1343,11 @@
       <c r="C47" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -1102,8 +1357,11 @@
       <c r="C48" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -1113,8 +1371,11 @@
       <c r="C49" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -1124,8 +1385,11 @@
       <c r="C50" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -1135,8 +1399,11 @@
       <c r="C51" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -1146,8 +1413,11 @@
       <c r="C52" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -1157,8 +1427,11 @@
       <c r="C53" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -1168,8 +1441,11 @@
       <c r="C54" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -1179,8 +1455,11 @@
       <c r="C55" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>45</v>
       </c>
@@ -1190,8 +1469,11 @@
       <c r="C56" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
@@ -1201,8 +1483,11 @@
       <c r="C57" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
@@ -1212,8 +1497,11 @@
       <c r="C58" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>46</v>
       </c>
@@ -1223,8 +1511,11 @@
       <c r="C59" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
@@ -1234,8 +1525,11 @@
       <c r="C60" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
@@ -1245,8 +1539,11 @@
       <c r="C61" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>48</v>
       </c>
@@ -1256,8 +1553,11 @@
       <c r="C62" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>49</v>
       </c>
@@ -1267,8 +1567,11 @@
       <c r="C63" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>49</v>
       </c>
@@ -1278,8 +1581,11 @@
       <c r="C64" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>49</v>
       </c>
@@ -1289,8 +1595,11 @@
       <c r="C65" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>49</v>
       </c>
@@ -1300,8 +1609,11 @@
       <c r="C66" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>49</v>
       </c>
@@ -1311,8 +1623,11 @@
       <c r="C67" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>49</v>
       </c>
@@ -1322,8 +1637,11 @@
       <c r="C68" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>49</v>
       </c>
@@ -1333,8 +1651,11 @@
       <c r="C69" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>49</v>
       </c>
@@ -1344,8 +1665,11 @@
       <c r="C70" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>49</v>
       </c>
@@ -1355,8 +1679,11 @@
       <c r="C71" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>50</v>
       </c>
@@ -1366,8 +1693,11 @@
       <c r="C72" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>50</v>
       </c>
@@ -1377,8 +1707,11 @@
       <c r="C73" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>50</v>
       </c>
@@ -1388,8 +1721,11 @@
       <c r="C74" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D74" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>50</v>
       </c>
@@ -1399,8 +1735,11 @@
       <c r="C75" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>50</v>
       </c>
@@ -1410,8 +1749,11 @@
       <c r="C76" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>50</v>
       </c>
@@ -1421,8 +1763,11 @@
       <c r="C77" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>50</v>
       </c>
@@ -1432,8 +1777,11 @@
       <c r="C78" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>50</v>
       </c>
@@ -1443,8 +1791,11 @@
       <c r="C79" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>50</v>
       </c>
@@ -1454,8 +1805,11 @@
       <c r="C80" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D80" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>51</v>
       </c>
@@ -1465,8 +1819,11 @@
       <c r="C81" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>51</v>
       </c>
@@ -1476,8 +1833,11 @@
       <c r="C82" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D82" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>51</v>
       </c>
@@ -1487,8 +1847,11 @@
       <c r="C83" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D83" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>52</v>
       </c>
@@ -1498,8 +1861,11 @@
       <c r="C84" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D84" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>52</v>
       </c>
@@ -1509,8 +1875,11 @@
       <c r="C85" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D85" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>52</v>
       </c>
@@ -1520,8 +1889,11 @@
       <c r="C86" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D86" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>53</v>
       </c>
@@ -1531,8 +1903,11 @@
       <c r="C87" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D87" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>55</v>
       </c>
@@ -1542,8 +1917,11 @@
       <c r="C88" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D88" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>56</v>
       </c>
@@ -1553,8 +1931,12 @@
       <c r="C89" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="D89" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>